<commit_message>
S28/G02: Signal backtest (EOD)
</commit_message>
<xml_diff>
--- a/docs/sprint_plans_codex.xlsx
+++ b/docs/sprint_plans_codex.xlsx
@@ -498,12 +498,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>planned</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Signal backtest (EOD) implemented: DSL + Top-N momentum ranking + presets + summary results.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-12-27T01:47:58</t>
+          <t>27/12/2025 02:30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S28/G03: Portfolio backtest v1 (target weights)
</commit_message>
<xml_diff>
--- a/docs/sprint_plans_codex.xlsx
+++ b/docs/sprint_plans_codex.xlsx
@@ -530,12 +530,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>planned</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Portfolio backtest v1 implemented: Target weights (EOD) with cadence/constraints/costs, equity+drawdown+actions.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-12-27T01:47:58</t>
+          <t>27/12/2025 03:04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S28/G04: Portfolio backtest v2 (rotation)
</commit_message>
<xml_diff>
--- a/docs/sprint_plans_codex.xlsx
+++ b/docs/sprint_plans_codex.xlsx
@@ -562,12 +562,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>planned</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Rotation backtest implemented: Top-N momentum (with optional eligible DSL) + compare overlay UI + tests.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-12-27T01:47:58</t>
+          <t>27/12/2025 03:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S28/G05: Portfolio backtest v3 (risk parity)
</commit_message>
<xml_diff>
--- a/docs/sprint_plans_codex.xlsx
+++ b/docs/sprint_plans_codex.xlsx
@@ -594,12 +594,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>planned</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Risk parity backtest implemented (ERC) with rolling window + bounds + UI presets + tests/help.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-12-27T01:47:58</t>
+          <t>27/12/2025 03:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S28/G06: Execution backtest (EOD friction model)
</commit_message>
<xml_diff>
--- a/docs/sprint_plans_codex.xlsx
+++ b/docs/sprint_plans_codex.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -626,12 +626,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>planned</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Execution backtest implemented: base portfolio run selection + ideal vs realistic fills (CLOSE vs NEXT_OPEN) with slippage/charges + comparison chart and API tests.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-12-27T01:47:58</t>
+          <t>27/12/2025 04:42</t>
         </is>
       </c>
     </row>

</xml_diff>